<commit_message>
* deleted unused files and modules
</commit_message>
<xml_diff>
--- a/src/input.xlsx
+++ b/src/input.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Offers.name</t>
   </si>
   <si>
-    <t xml:space="preserve">offers(vendor::price::currencyId::categoryId)</t>
+    <t xml:space="preserve">offers(vendor::price::currencyId::categoryId::id)</t>
   </si>
   <si>
     <t xml:space="preserve">offers.description</t>
@@ -58,13 +58,13 @@
     <t xml:space="preserve">122::Женские серебряные кольца</t>
   </si>
   <si>
-    <t xml:space="preserve">300::1::13</t>
+    <t xml:space="preserve">400::1::13</t>
   </si>
   <si>
     <t xml:space="preserve">Кольцо из серебра с куб. циркониями Ювелир центр 925 Damiani MINOU in OrO, 17.5 размер</t>
   </si>
   <si>
-    <t xml:space="preserve">Ювелир центр::160::UAH::122</t>
+    <t xml:space="preserve">Ювелир центр::160::UAH::122::2589</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;p&gt;Кольцо выполнено в классическом стиле известных ювелирных домов.&lt;/p&gt;
@@ -79,10 +79,10 @@
   <si>
     <t xml:space="preserve">Размер::17.5
 Металл::Серебро
-Камни::“Кубический цирконий“
-Металл::“Серебро 925°“
-Вес::“3.5 грамм“
-Доставка/Оплата::“Товар под заказ. Срок доставки до 7 дней. Предоплата 10%“</t>
+Камни::Кубический цирконий
+Металл::Серебро 925°
+Вес::3.5 грамм
+Доставка/Оплата::Товар под заказ. Срок доставки до 7 дней. Предоплата 10%</t>
   </si>
   <si>
     <t xml:space="preserve">http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4854.JPG
@@ -272,7 +272,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,7 +361,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
* corrected parser for use the correct data type
</commit_message>
<xml_diff>
--- a/src/input.xlsx
+++ b/src/input.xlsx
@@ -85,9 +85,9 @@
 Доставка/Оплата::Товар под заказ. Срок доставки до 7 дней. Предоплата 10%</t>
   </si>
   <si>
-    <t xml:space="preserve">http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4854.JPG
-http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4856.JPG
-http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4863.JPG</t>
+    <t xml:space="preserve">http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4854.jpg
+http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4856.jpg
+http://center-jeweler.com.ua/image/data/kolca11/watermarked — DSCN4863.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">http://center-jeweler.com.ua/serebro/kolca-1/kolco-serebro-925-damiani-minou-oro</t>
@@ -360,7 +360,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -423,7 +423,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="7" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="7" customFormat="true" ht="215.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -446,7 +446,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="10" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>17</v>

</xml_diff>